<commit_message>
Evolution of ODI Scores
</commit_message>
<xml_diff>
--- a/Results/median_score.xlsx
+++ b/Results/median_score.xlsx
@@ -13,7 +13,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -899,8 +898,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="600261632"/>
-        <c:axId val="152945216"/>
+        <c:axId val="595163136"/>
+        <c:axId val="577126400"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1184,11 +1183,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="172603392"/>
-        <c:axId val="152945792"/>
+        <c:axId val="595164160"/>
+        <c:axId val="577126976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="600261632"/>
+        <c:axId val="595163136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1197,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152945216"/>
+        <c:crossAx val="577126400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1206,7 +1205,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152945216"/>
+        <c:axId val="577126400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
@@ -1236,12 +1235,12 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="600261632"/>
+        <c:crossAx val="595163136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="152945792"/>
+        <c:axId val="577126976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,12 +1269,12 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172603392"/>
+        <c:crossAx val="595164160"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="172603392"/>
+        <c:axId val="595164160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,7 +1284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152945792"/>
+        <c:crossAx val="577126976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1529,56 +1528,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6705600" y="342900"/>
-          <a:ext cx="28575" cy="2771775"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Straight Connector 13"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4371975" y="342900"/>
           <a:ext cx="28575" cy="2771775"/>
         </a:xfrm>
         <a:prstGeom prst="line">

</xml_diff>